<commit_message>
Change hierarhy, add factoids, works on catalog
</commit_message>
<xml_diff>
--- a/data/Напольные конвекторы.xlsx
+++ b/data/Напольные конвекторы.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/santech/Documents/My/WebProjects/Heaton/heaton_/heaton/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84520336-5BC2-2049-9591-F71F614100C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D5D4CC-5FFF-C747-AEE6-8110541AB0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="4120" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{9B16654C-A221-B44A-BD15-4BFA61150284}"/>
+    <workbookView xWindow="6980" yWindow="4540" windowWidth="27240" windowHeight="16440" xr2:uid="{9B16654C-A221-B44A-BD15-4BFA61150284}"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="1" r:id="rId1"/>
@@ -904,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16D0F18-844B-F548-AB93-6464A8420166}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -972,7 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5F091B-3AD8-4145-BC5B-AF588F67BB8E}">
   <dimension ref="A1:K1837"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>

</xml_diff>